<commit_message>
Perfect Doctor Homework a
finished part a of the perfect doctor homework assignment.
</commit_message>
<xml_diff>
--- a/Exercises/Perfect_Doctor.xlsx
+++ b/Exercises/Perfect_Doctor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/UT-Causal-Inference/Exercises/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfperez\Documents\GitHub\UT-Causal-Inference\Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CA58D0-7573-924C-B041-64E4B1D15D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB3C0B5-5F3F-4327-9436-02A805A59DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="49340" windowHeight="28300" activeTab="1" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{083BD555-0A53-1B4B-AE70-5F7A5361EDB7}"/>
   </bookViews>
   <sheets>
     <sheet name="together" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -217,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +277,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -416,6 +424,8 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,24 +742,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F72EDE92-11F1-504D-AA85-77E1FD099BAB}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" customWidth="1"/>
+    <col min="8" max="8" width="23.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -768,18 +778,27 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>6</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="29">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>-4</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5">
+        <f>E2*C2 + (1-E2)*B2</f>
+        <v>6</v>
+      </c>
       <c r="H2" t="s">
         <v>32</v>
       </c>
@@ -787,105 +806,168 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="29">
         <v>8</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F13" si="1">E3*C3 + (1-E3)*B3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="29">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="F4" s="14"/>
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="H4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="29">
         <v>8</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="29">
         <v>5</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="F6" s="14"/>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
       <c r="H6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="29">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5">
         <v>2</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="29">
         <v>2</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="29">
         <v>1</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="F9" s="14"/>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="H9" t="s">
         <v>35</v>
       </c>
@@ -893,66 +975,102 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="29">
         <v>10</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="F10" s="14"/>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="I10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5">
         <v>2</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="29">
         <v>7</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="F11" s="14"/>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="I11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="5">
         <v>8</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="29">
         <v>4</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5">
         <v>2</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="29">
         <v>8</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>18</v>
       </c>
@@ -961,11 +1079,22 @@
       </c>
       <c r="C16" s="21"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <f>B17-C17</f>
+        <v>1.3428571428571425</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(F3,F5,F10,F11,F13)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(F2,F4,F6:F9,F12)</f>
+        <v>6.8571428571428568</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
@@ -985,19 +1114,37 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19"/>
+    <row r="20" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="15">
+        <f>AVERAGE(B3,B5,B10:B11,B13)</f>
+        <v>3</v>
+      </c>
+      <c r="B20" s="16">
+        <f>AVERAGE(B2,B4,B6:B9,B12)</f>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="C20" s="17">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D20" s="18">
+        <f>AVERAGE(D3,D5,D10:D11,D13)</f>
+        <v>5.2</v>
+      </c>
+      <c r="E20" s="18">
+        <f>AVERAGE(D12,D6:D9,D4,D2)</f>
+        <v>-3.2857142857142856</v>
+      </c>
+      <c r="F20" s="19">
+        <f>AVERAGE(D2:D13)</f>
+        <v>0.25</v>
+      </c>
       <c r="H20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>25</v>
       </c>
@@ -1009,7 +1156,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>41</v>
       </c>
@@ -1017,16 +1164,22 @@
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="F23" s="12">
+        <f>F20+A20-B20+(1-C20)*(D20-E20)</f>
+        <v>1.3428571428571425</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="B26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1037,13 +1190,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658F0CAF-38BA-064D-B720-EB93DBD0638C}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1243,7 @@
       </c>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1255,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1267,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1279,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1291,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1150,7 +1303,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1162,7 +1315,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1327,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1186,7 +1339,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1198,7 +1351,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1210,7 +1363,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1222,7 +1375,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1239,7 +1392,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1260,12 +1413,12 @@
         <v>13.428571428571429</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1282,7 +1435,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1296,20 +1449,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0224CB-C32E-2849-913B-D3BC1D805D51}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -1337,58 +1490,113 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>80</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="29">
         <v>81</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D2" s="7">
+        <f>C2-B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>E2*C2+(1-E2)*B2</f>
+        <v>81</v>
+      </c>
+      <c r="G2" s="12">
+        <f>G6-H6</f>
+        <v>-12.000000000000007</v>
+      </c>
+      <c r="H2" s="12">
+        <f>AVERAGE(E2:E13)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="12">
+        <f>AVERAGE(D2:D13)</f>
+        <v>-20.583333333333332</v>
+      </c>
+      <c r="J2" s="12">
+        <f>AVERAGE(D4,D6:D7,D10,D12:D13)</f>
+        <v>-9.1666666666666661</v>
+      </c>
+      <c r="K2" s="12">
+        <f>AVERAGE(D2:D3,D5,D8:D9,D11)</f>
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="5">
         <v>88</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="29">
         <v>46</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>-42</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">E3*C3+(1-E3)*B3</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
         <v>68</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="29">
         <v>33</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D4" s="7">
+        <f t="shared" si="0"/>
+        <v>-35</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5">
         <v>62</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="29">
         <v>77</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
       <c r="G5" s="8" t="s">
         <v>48</v>
       </c>
@@ -1402,126 +1610,221 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5">
         <v>71</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="29">
         <v>83</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="G6" s="12">
+        <f>AVERAGE(F2:F3,F5,F8:F9,F11)</f>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="H6" s="12">
+        <f>AVERAGE(F4,F6:F7,F10,F12:F13)</f>
+        <v>66.166666666666671</v>
+      </c>
+      <c r="I6" s="12">
+        <f>AVERAGE(B2:B3,B5,B8:B9,B11)</f>
+        <v>86.166666666666671</v>
+      </c>
+      <c r="J6" s="12">
+        <f>AVERAGE(B4,B6:B7,B10,B12:B13)</f>
+        <v>66.166666666666671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5">
         <v>61</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="29">
         <v>58</v>
       </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5">
         <v>100</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="29">
         <v>34</v>
       </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>-66</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="5">
         <v>94</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="29">
         <v>30</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>-64</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
       <c r="G9" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>51</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="29">
         <v>66</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="G10" s="12">
+        <f>I2+'homework part a'!I6-'homework part a'!J6+(1-'homework part a'!H2)*('homework part a'!K2-'homework part a'!J2)</f>
+        <v>-11.999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5">
         <v>93</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="29">
         <v>57</v>
       </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>-36</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="5">
         <v>73</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="29">
         <v>37</v>
       </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>-36</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5">
         <v>73</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="29">
         <v>65</v>
       </c>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="7">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1538,7 +1841,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1556,9 +1859,9 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1593,7 +1896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1610,7 +1913,7 @@
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1622,7 +1925,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1634,7 +1937,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1658,7 +1961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1977,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1686,7 +1989,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1698,7 +2001,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1713,7 +2016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1726,7 +2029,7 @@
       <c r="D10" s="7"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1738,7 +2041,7 @@
       </c>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1750,7 +2053,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1762,22 +2065,22 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1794,7 +2097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>47</v>
       </c>

</xml_diff>